<commit_message>
Fixed locator_args for list. Updated simple demo.
</commit_message>
<xml_diff>
--- a/demo/simple_demo.xlsx
+++ b/demo/simple_demo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="tr0001" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="55">
   <si>
     <t xml:space="preserve">tr_uuid:</t>
   </si>
@@ -175,6 +175,18 @@
   </si>
   <si>
     <t xml:space="preserve">Tass Sample Case B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locator_args</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q6a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">btnFormat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Color</t>
   </si>
 </sst>
 </file>
@@ -286,11 +298,11 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -352,12 +364,14 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.65234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="2" width="11.65"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="2" width="11.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="40.69"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="2" width="11.64"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -572,15 +586,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.65234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="2" width="11.65"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="2" width="11.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="28.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="28.34"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="2" width="11.64"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -628,6 +645,9 @@
       <c r="J2" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="K2" s="2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -813,6 +833,27 @@
       <c r="G12" s="3"/>
       <c r="I12" s="2" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="K13" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated demo. Updated imports for __main__ x2
</commit_message>
<xml_diff>
--- a/demo/simple_demo.xlsx
+++ b/demo/simple_demo.xlsx
@@ -96,7 +96,7 @@
     <t xml:space="preserve">selenium,load_file</t>
   </si>
   <si>
-    <t xml:space="preserve">tests/pages/page1.html</t>
+    <t xml:space="preserve">demo/demo-html/page1.html</t>
   </si>
   <si>
     <t xml:space="preserve">q2</t>
@@ -302,7 +302,7 @@
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -364,14 +364,16 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.65234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="2" width="11.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="40.69"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="2" width="11.64"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="4" style="2" width="11.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="29.59"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="2" width="11.64"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -589,7 +591,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.65234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -597,7 +599,9 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="2" width="11.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="28.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="28.34"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="2" width="11.64"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="2" width="11.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="38.9"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="2" width="11.64"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>